<commit_message>
new server: ftp without connection with DB
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
   <si>
     <t>Название команды</t>
   </si>
@@ -517,6 +517,9 @@
       </rPr>
       <t>(Поддерживается)</t>
     </r>
+  </si>
+  <si>
+    <t>Сервер (fast)+B2:C15E40C2:C10B2:C23B2:C30E40B2:C31</t>
   </si>
 </sst>
 </file>
@@ -932,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -946,52 +949,73 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1003,44 +1027,35 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1331,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,849 +1396,862 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="s">
+      <c r="E4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="20"/>
+    </row>
+    <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="F7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:10" ht="36" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="20"/>
+    </row>
+    <row r="24" spans="1:10" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
+      <c r="B26" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
+      <c r="B27" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="32"/>
+      <c r="B28" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+      <c r="D29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="C30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="19"/>
+    </row>
+    <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="33" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D33" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+      <c r="D35" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="19"/>
+    </row>
+    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="C36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="19"/>
+    </row>
+    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
+      <c r="D37" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="19"/>
+    </row>
+    <row r="38" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="32"/>
+      <c r="B38" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" ht="36" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="C38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26" t="s">
+      <c r="D39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
-    </row>
-    <row r="20" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="1:10" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:10" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="C40" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33" t="s">
+      <c r="E40" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G39" s="33"/>
-      <c r="H39" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J39" s="34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35" t="s">
+      <c r="G40" s="14"/>
+      <c r="H40" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="I40" s="35"/>
-      <c r="J40" s="36"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="J29:J38"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="D27:I27"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="J6:J9"/>
@@ -2240,19 +2268,6 @@
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="D15:I15"/>
     <mergeCell ref="A24:A28"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="J29:J38"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="J22:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>